<commit_message>
Se quita limpiador de filas repetidos de la funcion que muestra results paara que no haya desfase entre la tabal de result real y lo que se muestra. Ademas se agregan deshabilitadores de botones para el modelamiento.
</commit_message>
<xml_diff>
--- a/data/raw/comunas_descripcion.xlsx
+++ b/data/raw/comunas_descripcion.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\streamlit_app_clusters_crimen\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE8602B-FD78-4479-B281-988B6E76F060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8168BC-2B85-4069-BB5E-4F3202D7292E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38505" yWindow="-1080" windowWidth="31815" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-1200" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="descripciones_comunas" sheetId="1" r:id="rId1"/>
+    <sheet name="documentacion_descripciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -127,6 +128,21 @@
     <t xml:space="preserve">preferencia por comuna del transporte informal;
 terminalitos
 </t>
+  </si>
+  <si>
+    <t>zona residencial</t>
+  </si>
+  <si>
+    <t>zona educativa</t>
+  </si>
+  <si>
+    <t>zona de turismo</t>
+  </si>
+  <si>
+    <t>alto trafico</t>
+  </si>
+  <si>
+    <t>alto nivel de comercio entre las 2 y 7pm</t>
   </si>
 </sst>
 </file>
@@ -462,7 +478,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,6 +499,246 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23714016-EEE3-4C64-9D9B-B88005A42014}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>